<commit_message>
Mudanças no plano de projeto e configuração conforme a solicitação #17
</commit_message>
<xml_diff>
--- a/1-Gerência/1.04-Qualidade de Software/Definição Processo-Grupo3/Templates/Gerência de Projeto/[TEMPLATE] Planilha de gerenciamento dos riscos.xlsx
+++ b/1-Gerência/1.04-Qualidade de Software/Definição Processo-Grupo3/Templates/Gerência de Projeto/[TEMPLATE] Planilha de gerenciamento dos riscos.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucoes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="Status">#REF!</definedName>
     <definedName name="Urgencia">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -157,20 +157,20 @@
     <t>1 A 5</t>
   </si>
   <si>
-    <t>Mitigação</t>
-  </si>
-  <si>
-    <t>Plano de Contingência</t>
+    <t>Todos os riscos, independente da sua prioridade será monitorado semanalmente, de acordo</t>
+  </si>
+  <si>
+    <t>com a política organizacional para o processo de Gerência de Projeto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -224,6 +224,13 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -391,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -491,6 +498,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +720,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -746,6 +755,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -921,12 +931,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -936,7 +946,7 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -944,7 +954,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -954,7 +964,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
@@ -964,7 +974,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -972,7 +982,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
         <v>2</v>
@@ -984,7 +994,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="14.25">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -1000,7 +1010,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="25">
         <v>1</v>
@@ -1014,7 +1024,7 @@
       <c r="E7" s="34"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="14.25">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="35">
         <f t="shared" ref="B8:B9" si="0">B7+1</f>
@@ -1029,7 +1039,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="35">
         <f t="shared" si="0"/>
@@ -1040,7 +1050,7 @@
       <c r="E9" s="34"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="12"/>
@@ -1054,34 +1064,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="11"/>
       <c r="D1" s="12"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="15" t="s">
         <v>7</v>
@@ -1096,17 +1102,11 @@
         <v>13</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="18">
         <v>1</v>
@@ -1114,298 +1114,265 @@
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="20">
-        <f>IF(ISTEXT(D3),LEFT(D3,1),D3)*IF(ISTEXT(E3),LEFT(E3,1),E3)</f>
+      <c r="F3" s="20">
+        <f t="shared" ref="F3:F17" si="0">IF(ISTEXT(D3),LEFT(D3,1),D3)*IF(ISTEXT(E3),LEFT(E3,1),E3)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="21">
-        <f t="shared" ref="B4:B17" si="0">B3+1</f>
+        <f t="shared" ref="B4:B17" si="1">B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="20">
-        <f>IF(ISTEXT(D4),LEFT(D4,1),D4)*IF(ISTEXT(E4),LEFT(E4,1),E4)</f>
+      <c r="F4" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="B5" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="20">
-        <f>IF(ISTEXT(D5),LEFT(D5,1),D5)*IF(ISTEXT(E5),LEFT(E5,1),E5)</f>
+      <c r="F5" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="22"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="20">
-        <f>IF(ISTEXT(D6),LEFT(D6,1),D6)*IF(ISTEXT(E6),LEFT(E6,1),E6)</f>
+      <c r="F6" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="20">
-        <f>IF(ISTEXT(D7),LEFT(D7,1),D7)*IF(ISTEXT(E7),LEFT(E7,1),E7)</f>
+      <c r="F7" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="20">
-        <f>IF(ISTEXT(D8),LEFT(D8,1),D8)*IF(ISTEXT(E8),LEFT(E8,1),E8)</f>
+      <c r="F8" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="G8" s="22"/>
+      <c r="I8" s="47"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="20">
-        <f>IF(ISTEXT(D9),LEFT(D9,1),D9)*IF(ISTEXT(E9),LEFT(E9,1),E9)</f>
+      <c r="F9" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="20">
-        <f>IF(ISTEXT(D10),LEFT(D10,1),D10)*IF(ISTEXT(E10),LEFT(E10,1),E10)</f>
+      <c r="F10" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="20">
-        <f>IF(ISTEXT(D11),LEFT(D11,1),D11)*IF(ISTEXT(E11),LEFT(E11,1),E11)</f>
+      <c r="F11" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="20">
-        <f>IF(ISTEXT(D12),LEFT(D12,1),D12)*IF(ISTEXT(E12),LEFT(E12,1),E12)</f>
+      <c r="F12" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="20">
-        <f>IF(ISTEXT(D13),LEFT(D13,1),D13)*IF(ISTEXT(E13),LEFT(E13,1),E13)</f>
+      <c r="F13" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="20">
-        <f>IF(ISTEXT(D14),LEFT(D14,1),D14)*IF(ISTEXT(E14),LEFT(E14,1),E14)</f>
+      <c r="F14" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="20">
-        <f>IF(ISTEXT(D15),LEFT(D15,1),D15)*IF(ISTEXT(E15),LEFT(E15,1),E15)</f>
+      <c r="F15" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="20">
-        <f>IF(ISTEXT(D16),LEFT(D16,1),D16)*IF(ISTEXT(E16),LEFT(E16,1),E16)</f>
+      <c r="F16" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="20">
-        <f>IF(ISTEXT(D17),LEFT(D17,1),D17)*IF(ISTEXT(E17),LEFT(E17,1),E17)</f>
+      <c r="F17" s="20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="22"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H17">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F4:F17">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H17">
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="F4:F17">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H17">
-    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="F4:F17">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1413,28 +1380,31 @@
     <dataValidation type="list" showErrorMessage="1" sqref="D3:D17">
       <formula1>Probabilidade</formula1>
     </dataValidation>
-    <dataValidation type="list" showErrorMessage="1" sqref="E3:G17">
+    <dataValidation type="list" showErrorMessage="1" sqref="E3:E17">
       <formula1>Impacto</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1443,20 +1413,20 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="36">
         <f t="shared" ref="B3:B6" si="0">B4+1</f>
@@ -1483,7 +1453,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="36">
         <f t="shared" si="0"/>
@@ -1510,7 +1480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="36">
         <f t="shared" si="0"/>
@@ -1537,7 +1507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="36">
         <f t="shared" si="0"/>
@@ -1564,7 +1534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="29">
         <v>1</v>
@@ -1590,7 +1560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="14" t="s">
         <v>13</v>
@@ -1615,7 +1585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1624,24 +1594,24 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="38"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="39" t="s">
@@ -1652,7 +1622,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="42"/>
       <c r="C14" s="43" t="s">
@@ -1667,7 +1637,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="46" t="s">
@@ -1682,7 +1652,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1691,25 +1661,29 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1718,7 +1692,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1732,17 +1706,17 @@
     <mergeCell ref="C2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:G7">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:G7">
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:G7">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1751,12 +1725,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -1766,7 +1740,7 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1774,17 +1748,17 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="26" t="s">
         <v>16</v>
@@ -1802,7 +1776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="29" t="s">
         <v>18</v>
@@ -1814,7 +1788,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="31" t="s">
         <v>20</v>
@@ -1830,7 +1804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31" t="s">
@@ -1844,7 +1818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="31"/>
       <c r="C7" s="31" t="s">
@@ -1858,7 +1832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31" t="s">
@@ -1872,7 +1846,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -1884,7 +1858,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -1892,7 +1866,7 @@
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -1900,7 +1874,7 @@
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1908,7 +1882,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1916,7 +1890,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1924,7 +1898,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1932,7 +1906,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1940,7 +1914,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1948,7 +1922,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1956,7 +1930,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1964,7 +1938,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>

</xml_diff>